<commit_message>
added data of gastric and colorectal cancer
</commit_message>
<xml_diff>
--- a/staticfiles/Data/ColorectalCancer.xlsx
+++ b/staticfiles/Data/ColorectalCancer.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12555"/>
+    <workbookView windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="ColorectalCancer" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Country</t>
   </si>
@@ -211,19 +211,13 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>Opportunistic screening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  growing awareness and use of FIT in urban areas.</t>
+    <t>Opportunistic screening; growing awareness and use of FIT in urban areas.</t>
   </si>
   <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Opportunistic screening with FIT and colonoscopy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  some state-level programs.</t>
+    <t>Opportunistic screening with FIT and colonoscopy; some state-level programs.</t>
   </si>
   <si>
     <t>Argentina</t>
@@ -241,10 +235,7 @@
     <t>Colombia</t>
   </si>
   <si>
-    <t>National guidelines exist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  implementation mainly opportunistic or regional.</t>
+    <t>National guidelines exist; implementation mainly opportunistic or regional.</t>
   </si>
   <si>
     <t>United States</t>
@@ -274,100 +265,73 @@
     <t>Greece</t>
   </si>
   <si>
-    <t>No national program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  screening is opportunistic and awareness is growing.</t>
+    <t>No national program; screening is opportunistic and awareness is growing.</t>
   </si>
   <si>
     <t>Rwanda</t>
   </si>
   <si>
-    <t>No organized screening program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  very limited access to colonoscopy.</t>
+    <t>No organized screening program; very limited access to colonoscopy.</t>
   </si>
   <si>
     <t>Uganda</t>
   </si>
   <si>
-    <t>No formal program</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  screening extremely limited.</t>
+    <t>No formal program; screening extremely limited.</t>
   </si>
   <si>
     <t>Serbia</t>
   </si>
   <si>
-    <t>National FIT-based program implemented</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  colonoscopy for positive cases.</t>
+    <t>National FIT-based program implemented; colonoscopy for positive cases.</t>
   </si>
   <si>
     <t>Saudi Arabia</t>
   </si>
   <si>
-    <t xml:space="preserve">  opportunistic colonoscopy screening in urban hospitals.</t>
+    <t>No national program; opportunistic colonoscopy screening in urban hospitals.</t>
   </si>
   <si>
     <t>UAE</t>
   </si>
   <si>
-    <t>Opportunistic screening available in major hospitals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  no structured national program yet.</t>
+    <t>Opportunistic screening available in major hospitals; no structured national program yet.</t>
   </si>
   <si>
     <t>Syria</t>
   </si>
   <si>
-    <t>No colorectal cancer screening program</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> infrastructure severely impacted.</t>
+    <t>No colorectal cancer screening program;  infrastructure severely impacted.</t>
   </si>
   <si>
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Opportunistic FIT or colonoscopy in private hospitals</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> no national program.</t>
+    <t>Opportunistic FIT or colonoscopy in private hospitals; no national program.</t>
   </si>
   <si>
     <t>Vietnam</t>
   </si>
   <si>
-    <t>Opportunistic testing in urban centers</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pilot programs exist but no national policy.</t>
+    <t>Opportunistic testing in urban centers; pilot programs exist but no national policy.</t>
   </si>
   <si>
     <t>Philippines</t>
   </si>
   <si>
-    <t xml:space="preserve"> some NGO-driven and private hospital initiatives.</t>
+    <t>No organized screening program; some NGO-driven and private hospital initiatives.</t>
   </si>
   <si>
     <t>Russia</t>
   </si>
   <si>
-    <t>No national screening program</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> opportunistic colonoscopy available in major urban centers.</t>
+    <t>No national screening program; opportunistic colonoscopy available in major urban centers.</t>
   </si>
   <si>
     <t>Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve"> FIT/colonoscopy opportunistically</t>
+    <t>No national program; FIT/colonoscopy opportunistically</t>
   </si>
 </sst>
 </file>
@@ -375,10 +339,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -397,6 +361,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -405,37 +377,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -451,14 +393,52 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -473,17 +453,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -495,15 +475,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,22 +492,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -542,19 +506,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,61 +620,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,37 +638,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,43 +662,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,11 +700,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -777,44 +756,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -833,147 +777,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1306,13 +1270,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:W43"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.2" defaultRowHeight="15"/>
+  <cols>
+    <col min="22" max="22" width="83.7" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
@@ -2810,7 +2777,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -2877,13 +2844,10 @@
       <c r="V23" t="s">
         <v>65</v>
       </c>
-      <c r="W23" t="s">
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23">
-      <c r="A24" t="s">
-        <v>67</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -2946,15 +2910,12 @@
         <v>3</v>
       </c>
       <c r="V24" t="s">
-        <v>68</v>
-      </c>
-      <c r="W24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:22">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -3017,12 +2978,12 @@
         <v>3</v>
       </c>
       <c r="V25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:22">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -3085,12 +3046,12 @@
         <v>2</v>
       </c>
       <c r="V26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -3153,15 +3114,12 @@
         <v>2</v>
       </c>
       <c r="V27" t="s">
-        <v>75</v>
-      </c>
-      <c r="W27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -3224,12 +3182,12 @@
         <v>2</v>
       </c>
       <c r="V28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -3292,12 +3250,12 @@
         <v>2</v>
       </c>
       <c r="V29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:22">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -3360,12 +3318,12 @@
         <v>3</v>
       </c>
       <c r="V30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -3428,12 +3386,12 @@
         <v>3</v>
       </c>
       <c r="V31" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -3496,15 +3454,12 @@
         <v>3</v>
       </c>
       <c r="V32" t="s">
-        <v>86</v>
-      </c>
-      <c r="W32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3567,15 +3522,12 @@
         <v>1</v>
       </c>
       <c r="V33" t="s">
-        <v>89</v>
-      </c>
-      <c r="W33" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3638,15 +3590,12 @@
         <v>1</v>
       </c>
       <c r="V34" t="s">
-        <v>92</v>
-      </c>
-      <c r="W34" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B35">
         <v>3</v>
@@ -3709,15 +3658,12 @@
         <v>2</v>
       </c>
       <c r="V35" t="s">
-        <v>95</v>
-      </c>
-      <c r="W35" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -3780,15 +3726,12 @@
         <v>3</v>
       </c>
       <c r="V36" t="s">
-        <v>86</v>
-      </c>
-      <c r="W36" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -3851,15 +3794,12 @@
         <v>3</v>
       </c>
       <c r="V37" t="s">
-        <v>100</v>
-      </c>
-      <c r="W37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -3922,15 +3862,12 @@
         <v>1</v>
       </c>
       <c r="V38" t="s">
-        <v>103</v>
-      </c>
-      <c r="W38" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B39">
         <v>2</v>
@@ -3993,15 +3930,12 @@
         <v>2</v>
       </c>
       <c r="V39" t="s">
-        <v>106</v>
-      </c>
-      <c r="W39" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B40">
         <v>2</v>
@@ -4064,15 +3998,12 @@
         <v>2</v>
       </c>
       <c r="V40" t="s">
-        <v>109</v>
-      </c>
-      <c r="W40" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:22">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -4135,15 +4066,12 @@
         <v>2</v>
       </c>
       <c r="V41" t="s">
-        <v>89</v>
-      </c>
-      <c r="W41" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:22">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B42">
         <v>3</v>
@@ -4206,15 +4134,12 @@
         <v>3</v>
       </c>
       <c r="V42" t="s">
-        <v>114</v>
-      </c>
-      <c r="W42" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:22">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -4277,10 +4202,7 @@
         <v>2</v>
       </c>
       <c r="V43" t="s">
-        <v>86</v>
-      </c>
-      <c r="W43" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>